<commit_message>
Sigi-9: Find rows by headers
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\source\repos\SigiDoc\ExcelToXMLConverter\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugovasko/repos/SigiDoc/ExcelToXMLConverter/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E85470-1090-44A4-B244-9785993942B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D1F82C-F176-884D-86A0-DC6DDC72391D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
   <si>
     <t>SEAL ID</t>
   </si>
@@ -481,6 +481,27 @@
   </si>
   <si>
     <t>Varna</t>
+  </si>
+  <si>
+    <t>This is a seal title</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Shaw</t>
+  </si>
+  <si>
+    <t>Ivanov, 2017, 32, p.47</t>
+  </si>
+  <si>
+    <t>TM_98</t>
+  </si>
+  <si>
+    <t>0099</t>
+  </si>
+  <si>
+    <t>0098</t>
   </si>
 </sst>
 </file>
@@ -547,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -557,6 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,38 +961,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ61"/>
+  <dimension ref="A1:AMI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="B15" sqref="B15"/>
+      <selection pane="topRight" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="39" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" customWidth="1"/>
-    <col min="3" max="1024" width="11.5703125" style="2"/>
+    <col min="2" max="2" width="45.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
+    <col min="4" max="1023" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -978,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -986,7 +1015,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -994,7 +1023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1002,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1010,7 +1039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1018,22 +1047,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1041,7 +1070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1049,12 +1078,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1062,7 +1091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1192,7 +1221,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
@@ -1200,7 +1229,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
@@ -1208,7 +1237,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1216,7 +1245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1224,7 +1253,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
@@ -1232,7 +1261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
@@ -1240,7 +1269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
@@ -1248,7 +1277,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
@@ -1256,7 +1285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
@@ -1264,7 +1293,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -1272,7 +1301,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -1280,7 +1309,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
@@ -1288,15 +1317,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>65</v>
       </c>
@@ -1304,7 +1336,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
@@ -1312,7 +1344,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
         <v>67</v>
       </c>
@@ -1320,7 +1352,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1328,7 +1360,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>70</v>
       </c>
@@ -1336,12 +1368,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
@@ -1349,7 +1381,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>75</v>
       </c>
@@ -1357,17 +1389,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
@@ -1375,44 +1407,59 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:3" ht="14">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="2">
-        <v>99</v>
+      <c r="B61" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sigi-9: Generate filename and sequence number from seal id
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugovasko/repos/SigiDoc/ExcelToXMLConverter/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\source\repos\SigiDoc\ExcelToXMLConverter\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D1F82C-F176-884D-86A0-DC6DDC72391D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75AED02-65B6-4833-81ED-89EA083DB51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="112">
   <si>
     <t>SEAL ID</t>
   </si>
@@ -471,15 +471,6 @@
     <t>Petrov</t>
   </si>
   <si>
-    <t>Filename</t>
-  </si>
-  <si>
-    <t>TM_99</t>
-  </si>
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
     <t>Varna</t>
   </si>
   <si>
@@ -495,13 +486,16 @@
     <t>Ivanov, 2017, 32, p.47</t>
   </si>
   <si>
-    <t>TM_98</t>
-  </si>
-  <si>
-    <t>0099</t>
-  </si>
-  <si>
-    <t>0098</t>
+    <t>Another great title</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Kent</t>
+  </si>
+  <si>
+    <t>Another Edition</t>
   </si>
 </sst>
 </file>
@@ -568,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,7 +572,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,23 +954,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI61"/>
+  <dimension ref="A1:AMI59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A24" sqref="A24"/>
-      <selection pane="topRight" activeCell="C62" sqref="C62"/>
+      <selection pane="topRight" activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="39" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
-    <col min="4" max="1023" width="11.5" style="2"/>
+    <col min="2" max="2" width="45.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
+    <col min="5" max="1023" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -987,8 +981,11 @@
       <c r="C1" s="2">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -998,8 +995,11 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -1047,22 +1047,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -1078,12 +1078,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1221,7 +1221,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>50</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>56</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>58</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>63</v>
       </c>
@@ -1325,10 +1325,13 @@
         <v>64</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>107</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>65</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>67</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>70</v>
       </c>
@@ -1368,12 +1371,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>75</v>
       </c>
@@ -1389,17 +1392,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
@@ -1407,7 +1410,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14">
+    <row r="57" spans="1:4">
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
@@ -1415,10 +1418,13 @@
         <v>98</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>104</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
@@ -1426,10 +1432,13 @@
         <v>101</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>105</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -1437,29 +1446,10 @@
         <v>102</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sigi-9: Adding more keys in dictionary
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugovasko/repos/SigiDoc/ExcelToXMLConverter/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227FADD0-52FB-4148-ACB5-99BA1670D609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F85516-42A1-7543-A00F-22D0733CED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="156">
   <si>
     <t>SEAL ID</t>
   </si>
@@ -183,21 +183,12 @@
     <t>ACQUISITION</t>
   </si>
   <si>
-    <t>Some info here11</t>
-  </si>
-  <si>
     <t>PREVIOUS LOCATIONS</t>
   </si>
   <si>
-    <t>Some info here10</t>
-  </si>
-  <si>
     <t>MODERN OBSERVATIONS</t>
   </si>
   <si>
-    <t>Some info here9</t>
-  </si>
-  <si>
     <t>OBVERSE LAYOUT OF FIELD</t>
   </si>
   <si>
@@ -210,21 +201,12 @@
     <t>OBVERSE MATRIX</t>
   </si>
   <si>
-    <t>Some info here8</t>
-  </si>
-  <si>
     <t>OBVERSE ICONOGRAPHY</t>
   </si>
   <si>
-    <t>Some info here7</t>
-  </si>
-  <si>
     <t>OBVERSE DECORATION</t>
   </si>
   <si>
-    <t>Some info here6</t>
-  </si>
-  <si>
     <t>REVERSE LAYOUT FIELD</t>
   </si>
   <si>
@@ -234,21 +216,12 @@
     <t>REVERSE MATRIX</t>
   </si>
   <si>
-    <t>Some info here</t>
-  </si>
-  <si>
     <t>REVERSE ICONOGRAPHY</t>
   </si>
   <si>
-    <t>Some info here1</t>
-  </si>
-  <si>
     <t>REVERSE DECORATION</t>
   </si>
   <si>
-    <t>Some info here2</t>
-  </si>
-  <si>
     <t>LANGUAGE(S)</t>
   </si>
   <si>
@@ -261,28 +234,13 @@
     <t>Jordanov, 2011, 54, p. 26</t>
   </si>
   <si>
-    <t>Ivanov, 2017, 32, p.47</t>
-  </si>
-  <si>
-    <t>Another Edition</t>
-  </si>
-  <si>
     <t>COMMENTARY ON EDITION(S)</t>
   </si>
   <si>
-    <t>Some info here3</t>
-  </si>
-  <si>
     <t>PARALLEL(S)</t>
   </si>
   <si>
-    <t>Some info here4</t>
-  </si>
-  <si>
     <t>COMMENTARY ON PARALLEL(S)</t>
-  </si>
-  <si>
-    <t>Some info here5</t>
   </si>
   <si>
     <t>EDITION INTERPRETIVE</t>
@@ -456,56 +414,227 @@
     <t>BIBLIOGRAPHY</t>
   </si>
   <si>
-    <t>A lot text here</t>
-  </si>
-  <si>
     <t>TITLE</t>
   </si>
   <si>
-    <t>Seal of Somebody from somewhere</t>
-  </si>
-  <si>
-    <t>This is a seal title</t>
-  </si>
-  <si>
-    <t>Another great title</t>
-  </si>
-  <si>
     <t>EDITOR FORENAME</t>
   </si>
   <si>
     <t>Ivan</t>
   </si>
   <si>
-    <t>Steve</t>
-  </si>
-  <si>
-    <t>Clark</t>
-  </si>
-  <si>
     <t>EDITOR SURNAME</t>
   </si>
   <si>
     <t>Petrov</t>
   </si>
   <si>
-    <t>Shaw</t>
-  </si>
-  <si>
-    <t>Kent</t>
-  </si>
-  <si>
-    <t>768-985</t>
-  </si>
-  <si>
-    <t>846-685</t>
+    <t>ТИП</t>
+  </si>
+  <si>
+    <t>Двустранна легенда</t>
+  </si>
+  <si>
+    <t>Печат</t>
+  </si>
+  <si>
+    <t>СигиДок Айди: 13</t>
+  </si>
+  <si>
+    <t>ОФОРМЛЕНИЕ</t>
+  </si>
+  <si>
+    <t>МАТРИЦА (ПЕЧАТ)</t>
+  </si>
+  <si>
+    <t>ОТПЕЧАТЪК</t>
+  </si>
+  <si>
+    <t>МАТЕРИАЛ</t>
+  </si>
+  <si>
+    <t>Оригинален</t>
+  </si>
+  <si>
+    <t>Олово</t>
+  </si>
+  <si>
+    <t>НАЧИН НА ИЗРАБОТВАНЕ</t>
+  </si>
+  <si>
+    <t>Ударен</t>
+  </si>
+  <si>
+    <t>КОНТРАМАРКИ</t>
+  </si>
+  <si>
+    <t>Няма</t>
+  </si>
+  <si>
+    <t>ОСОБЕНОСТИ НА БУКВИТЕ</t>
+  </si>
+  <si>
+    <t>ФОРМА НА ЯДРОТО</t>
+  </si>
+  <si>
+    <t>Кръгъл</t>
+  </si>
+  <si>
+    <t>СЪВРЕМЕННО СЪСТОЯНИЕ</t>
+  </si>
+  <si>
+    <t>Счупен; корозирал</t>
+  </si>
+  <si>
+    <t>КРИТЕРИИ ЗА ДАТИРАНЕ</t>
+  </si>
+  <si>
+    <t>Буквено означение</t>
+  </si>
+  <si>
+    <t>АЛТЕРНАТИВНА ДАТИРОВКА</t>
+  </si>
+  <si>
+    <t>КОНТЕКСТ НА ПЕЧАТА</t>
+  </si>
+  <si>
+    <t>ИЗДАТЕЛ (СОБСТВЕНИК НА ПЕЧАТА)</t>
+  </si>
+  <si>
+    <t>СФЕРА НА ДЕЙНОСТ НА ИЗДАТЕЛЯ (СОБСТВЕНИКА НА ПЕЧАТА)</t>
+  </si>
+  <si>
+    <t>МЯСТО НА ИЗРАБОТКА</t>
+  </si>
+  <si>
+    <t>МЕСТОНАМИРАНЕ</t>
+  </si>
+  <si>
+    <t>ОБСТОЯТЕЛСТВА НА НАМИРАНЕ</t>
+  </si>
+  <si>
+    <t>СЪВРЕМЕННО СЕЛИЩЕ, ДО КОЕТО Е ОТКРИТ ПЕЧАТЪТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">МЯСТО НА СЪХРАНЕНИЕ </t>
+  </si>
+  <si>
+    <t>СПОСОБ НА ПРИДОБИВАНЕ</t>
+  </si>
+  <si>
+    <t>ПРЕДИШНО МЕСТОСЪХРАНЕНИЕ</t>
+  </si>
+  <si>
+    <t>СЪВРЕМЕННИ НАБЛЮДЕНИЯ</t>
+  </si>
+  <si>
+    <t>ОФОРМЛЕНИЕ НА ЛИЦЕВАТА СТРАНА</t>
+  </si>
+  <si>
+    <t>ЛИЦЕВ ПЕЧАТ / ЛИЦЕВА МАТРИЦА</t>
+  </si>
+  <si>
+    <t>ИКОНОГРАФИЯ НА АВЕРСА</t>
+  </si>
+  <si>
+    <t>ДЕКОРАТИВНИ ЕЛЕМЕНТИ НА АВЕРСА</t>
+  </si>
+  <si>
+    <t>ОФОРМЛЕНИЕ НА ОБРАТНАТА СТРАНА</t>
+  </si>
+  <si>
+    <t>РЕВЕРСЕН ПЕЧАТ / РЕВЕРС НА МАТРИЦА</t>
+  </si>
+  <si>
+    <t>ИКОНОГРАФИЯ НА РЕВЕРСА</t>
+  </si>
+  <si>
+    <t>ДЕКОРАТИВНИ ЕЛЕМЕНТИ НА РЕВЕРСА</t>
+  </si>
+  <si>
+    <t>ЕЗИК (ЕЗИЦИ)</t>
+  </si>
+  <si>
+    <t>КОМЕНТАР НА ПУБЛИКАЦИИТЕ</t>
+  </si>
+  <si>
+    <t>ПАРАЛЕЛ (ПАРАЛЕЛИ)</t>
+  </si>
+  <si>
+    <t>КОМЕНТАР НА ПАРАЛЕЛИТЕ</t>
+  </si>
+  <si>
+    <t>ИНТЕРПРЕТАТИВНО ИЗДАНИЕ</t>
+  </si>
+  <si>
+    <t>ДИПЛОМАТИЧНО ИЗДАНИЕ</t>
+  </si>
+  <si>
+    <t>КРИТИЧЕН АПАРАТ</t>
+  </si>
+  <si>
+    <t>НАДПИСИ</t>
+  </si>
+  <si>
+    <t>ПРЕВОД НА НАДПИСИТЕ</t>
+  </si>
+  <si>
+    <t>КОМЕНТАР НА НАДПИСИТЕ</t>
+  </si>
+  <si>
+    <t>БЕЛЕЖКИ ПОД ЛИНИЯ</t>
+  </si>
+  <si>
+    <t>БИБЛИОГРАФИЯ</t>
+  </si>
+  <si>
+    <t>ЗАГЛАВИЕ</t>
+  </si>
+  <si>
+    <t>СОБСТВЕНО ИМЕ НА РЕДАКТОРА</t>
+  </si>
+  <si>
+    <t>ФАМИЛНО ИМЕ НА РЕДАКТОРА</t>
+  </si>
+  <si>
+    <t>Иван</t>
+  </si>
+  <si>
+    <t>Петров</t>
+  </si>
+  <si>
+    <t>Заглавие на печата</t>
+  </si>
+  <si>
+    <t>Title of the seal</t>
+  </si>
+  <si>
+    <t>Централна администрация</t>
+  </si>
+  <si>
+    <t>Синезиос</t>
+  </si>
+  <si>
+    <t>Гражданска</t>
+  </si>
+  <si>
+    <t>Варна</t>
+  </si>
+  <si>
+    <t>Неизвестни</t>
+  </si>
+  <si>
+    <t>България</t>
+  </si>
+  <si>
+    <t>БАН</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -521,6 +650,13 @@
     <font>
       <sz val="10"/>
       <name val="Athena Ruby"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -565,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -575,6 +711,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,507 +1094,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMI59"/>
+  <dimension ref="A1:AMI105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B21" sqref="B21"/>
+      <selection pane="topRight" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="39" style="1" customWidth="1"/>
+    <col min="1" max="1" width="54.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="45.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
     <col min="5" max="1023" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>99</v>
       </c>
-      <c r="C1" s="2">
-        <v>98</v>
-      </c>
-      <c r="D1" s="2">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B12" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="1" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2" t="s">
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
+      <c r="B36" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
+    <row r="38" spans="1:2">
+      <c r="A38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
+    <row r="40" spans="1:2">
+      <c r="A40" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B43" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
+    <row r="44" spans="1:2">
+      <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
+    <row r="45" spans="1:2">
+      <c r="A45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
+    <row r="47" spans="1:2">
+      <c r="A47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
+    <row r="51" spans="1:2">
+      <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="2" t="s">
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
+    <row r="54" spans="1:2">
+      <c r="A54" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="2" t="s">
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="2" t="s">
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
+      <c r="B59" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="2" t="s">
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="3">
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
+    <row r="69" spans="1:2">
+      <c r="A69" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="2" t="s">
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
+    <row r="72" spans="1:2">
+      <c r="A72" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="2" t="s">
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1" t="s">
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="2" t="s">
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="1" t="s">
+    <row r="79" spans="1:2">
+      <c r="A79" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="2" t="s">
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="1" t="s">
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="1" t="s">
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1" t="s">
+    <row r="87" spans="1:2">
+      <c r="A87" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="2" t="s">
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="2" t="s">
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="2" t="s">
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="1" t="s">
+    <row r="95" spans="1:2">
+      <c r="A95" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="2" t="s">
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="1" t="s">
+    <row r="99" spans="1:2">
+      <c r="A99" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="14">
+      <c r="A100" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B100" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="14">
+      <c r="A101" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1" t="s">
+      <c r="B102" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B49" s="2" t="s">
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="1" t="s">
+      <c r="B104" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="14">
-      <c r="A57" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>110</v>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sigi-9: Fix typo in obverse
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugovasko/repos/SigiDoc/ExcelToXMLConverter/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\source\repos\SigiDoc\ExcelToXMLConverter\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F85516-42A1-7543-A00F-22D0733CED7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EE6540-027D-4C25-8E0E-9A56A24AF873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="176">
   <si>
     <t>SEAL ID</t>
   </si>
@@ -462,9 +462,6 @@
     <t>НАЧИН НА ИЗРАБОТВАНЕ</t>
   </si>
   <si>
-    <t>Ударен</t>
-  </si>
-  <si>
     <t>КОНТРАМАРКИ</t>
   </si>
   <si>
@@ -603,12 +600,6 @@
     <t>Петров</t>
   </si>
   <si>
-    <t>Заглавие на печата</t>
-  </si>
-  <si>
-    <t>Title of the seal</t>
-  </si>
-  <si>
     <t>Централна администрация</t>
   </si>
   <si>
@@ -628,6 +619,75 @@
   </si>
   <si>
     <t>БАН</t>
+  </si>
+  <si>
+    <t>“1”/&gt;ΘΕΟ “2”/&gt;ΤΟΚΕβΟ “3”/&gt;ηθιςυν “4”/&gt;εςιΩ - “1”/&gt;...β “2”/&gt;ΙΚ…ΑΡ “3”/&gt;ιΩ.βΑΙ “4”/&gt;Ουλος</t>
+  </si>
+  <si>
+    <t>SigiDoc ID: 11</t>
+  </si>
+  <si>
+    <t>СигиДок Айди:  Айди: 11</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Злато</t>
+  </si>
+  <si>
+    <t>Струг</t>
+  </si>
+  <si>
+    <t>Intact; corroded</t>
+  </si>
+  <si>
+    <t>Цялостен; корозирал</t>
+  </si>
+  <si>
+    <t>10th-11th C.</t>
+  </si>
+  <si>
+    <t>837-894</t>
+  </si>
+  <si>
+    <t>Plovdiv</t>
+  </si>
+  <si>
+    <t>Пловдив</t>
+  </si>
+  <si>
+    <t>Legend of 6 lines</t>
+  </si>
+  <si>
+    <t>Seal of Synesios</t>
+  </si>
+  <si>
+    <t>Печат на Синезиос</t>
+  </si>
+  <si>
+    <t>Constantine IV</t>
+  </si>
+  <si>
+    <t>Константин IV</t>
+  </si>
+  <si>
+    <t>Печат на Константин IV</t>
+  </si>
+  <si>
+    <t>Petar</t>
+  </si>
+  <si>
+    <t>Петър</t>
+  </si>
+  <si>
+    <t>Иванов</t>
+  </si>
+  <si>
+    <t>Ivanov</t>
+  </si>
+  <si>
+    <t>NAIM-BAN 48</t>
   </si>
 </sst>
 </file>
@@ -1096,714 +1156,885 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B99" sqref="B99"/>
+      <selection pane="topRight" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="54.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
-    <col min="5" max="1023" width="11.5" style="2"/>
+    <col min="1" max="1" width="54.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="87.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
+    <col min="5" max="1023" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>158</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>146</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>147</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>148</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>149</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B43" s="2">
         <v>2017</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" s="2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>150</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>151</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>152</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B59" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B68" s="3">
         <v>22</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
         <v>72</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="14">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="14">
+        <v>166</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>167</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="C102" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>144</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
       <c r="A104" s="5" t="s">
         <v>87</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="C104" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sigi-9: Improve bg translation for seal in excel
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\source\repos\SigiDoc\ExcelToXMLConverter\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugovasko/repos/SigiDoc/ExcelToXMLConverter/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EE6540-027D-4C25-8E0E-9A56A24AF873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3FE2E4-B2E2-BC44-9ADE-A334FE838382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="177">
   <si>
     <t>SEAL ID</t>
   </si>
@@ -688,6 +688,9 @@
   </si>
   <si>
     <t>NAIM-BAN 48</t>
+  </si>
+  <si>
+    <t>Seal of Constantine IV</t>
   </si>
 </sst>
 </file>
@@ -1158,16 +1161,16 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C78" sqref="C78"/>
+      <selection pane="topRight" activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="87.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="87.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
-    <col min="5" max="1023" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
+    <col min="5" max="1023" width="11.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1971,7 +1974,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" ht="14">
       <c r="A100" s="5" t="s">
         <v>84</v>
       </c>
@@ -1979,10 +1982,10 @@
         <v>166</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="14">
       <c r="A101" s="5" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
Sigi-11: Improve XML convertor script structure
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugovasko/repos/SigiDoc/ExcelToXMLConverter/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\source\repos\SigiDoc\ExcelToXMLConverter\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B4504C-290A-B84A-8717-8D97CF449654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4584F13-AC5B-4EB0-AD5F-04DDD526F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="90" windowWidth="25650" windowHeight="15270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,9 +438,6 @@
     <t>Печат</t>
   </si>
   <si>
-    <t>СигиДок Айди: 13</t>
-  </si>
-  <si>
     <t>ОФОРМЛЕНИЕ</t>
   </si>
   <si>
@@ -627,9 +624,6 @@
     <t>SigiDoc ID: 11</t>
   </si>
   <si>
-    <t>СигиДок Айди:  Айди: 11</t>
-  </si>
-  <si>
     <t>Gold</t>
   </si>
   <si>
@@ -693,15 +687,9 @@
     <t>Seal of Constantine IV</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
     <t>42.698334</t>
   </si>
   <si>
-    <t>longitude</t>
-  </si>
-  <si>
     <t>23.319941</t>
   </si>
   <si>
@@ -709,6 +697,18 @@
   </si>
   <si>
     <t>24.742168</t>
+  </si>
+  <si>
+    <t>LATITUDE</t>
+  </si>
+  <si>
+    <t>LONGITUDE</t>
+  </si>
+  <si>
+    <t>СигиДок ИД: 13</t>
+  </si>
+  <si>
+    <t>СигиДок ИД: 11</t>
   </si>
 </sst>
 </file>
@@ -1177,18 +1177,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B107" sqref="B107"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="54.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="87.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="87.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
-    <col min="5" max="1023" width="11.5" style="2"/>
+    <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
+    <col min="5" max="1023" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1237,7 +1237,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>90</v>
@@ -1254,18 +1254,18 @@
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>155</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1281,13 +1281,13 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1298,18 +1298,18 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1362,13 +1362,13 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1384,13 +1384,13 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1400,7 +1400,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1416,13 +1416,13 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1433,18 +1433,18 @@
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -1455,7 +1455,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1466,7 +1466,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1482,13 +1482,13 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1498,7 +1498,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -1514,13 +1514,13 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1531,18 +1531,18 @@
         <v>36</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1558,13 +1558,13 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1574,7 +1574,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1585,18 +1585,18 @@
         <v>41</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1623,13 +1623,13 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1645,13 +1645,13 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1667,13 +1667,13 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1684,7 +1684,7 @@
         <v>50</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1694,7 +1694,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1704,7 +1704,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1714,7 +1714,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1725,12 +1725,12 @@
         <v>55</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1751,7 +1751,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1761,7 +1761,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1771,7 +1771,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1782,12 +1782,12 @@
         <v>55</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -1808,7 +1808,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1818,7 +1818,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1828,7 +1828,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1844,7 +1844,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -1865,7 +1865,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -1875,7 +1875,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1885,7 +1885,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1901,7 +1901,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1912,12 +1912,12 @@
         <v>75</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1927,7 +1927,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="90" spans="1:3">
@@ -1943,7 +1943,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -1959,7 +1959,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:3">
@@ -1969,7 +1969,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:3">
@@ -1979,7 +1979,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:3">
@@ -1989,29 +1989,29 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="14">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
         <v>84</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="14">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -2022,18 +2022,18 @@
         <v>86</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:3">
@@ -2044,45 +2044,45 @@
         <v>88</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="C106" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="C107" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Sigi-11: Remove coordinates to json logic from C# script
</commit_message>
<xml_diff>
--- a/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
+++ b/ExcelToXMLConverter/resources/SIGIDOC CELLS ENG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugov\source\repos\SigiDoc\ExcelToXMLConverter\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4584F13-AC5B-4EB0-AD5F-04DDD526F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0459F3D9-28A1-46F9-A492-9E699BE3FF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="90" windowWidth="25650" windowHeight="15270" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="180">
   <si>
     <t>SEAL ID</t>
   </si>
@@ -687,28 +687,19 @@
     <t>Seal of Constantine IV</t>
   </si>
   <si>
-    <t>42.698334</t>
-  </si>
-  <si>
-    <t>23.319941</t>
-  </si>
-  <si>
-    <t>42.136097</t>
-  </si>
-  <si>
-    <t>24.742168</t>
-  </si>
-  <si>
-    <t>LATITUDE</t>
-  </si>
-  <si>
-    <t>LONGITUDE</t>
-  </si>
-  <si>
     <t>СигиДок ИД: 13</t>
   </si>
   <si>
     <t>СигиДок ИД: 11</t>
+  </si>
+  <si>
+    <t>42.136097, 24.742168</t>
+  </si>
+  <si>
+    <t>42.698334, 23.319941</t>
+  </si>
+  <si>
+    <t>COORDINATES</t>
   </si>
 </sst>
 </file>
@@ -1177,9 +1168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMI107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C7" sqref="C7"/>
+      <selection pane="topRight" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -1262,10 +1253,10 @@
         <v>93</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2066,19 +2057,11 @@
         <v>177</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>176</v>
-      </c>
+      <c r="A107" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>